<commit_message>
add table for omics data set in supp data
</commit_message>
<xml_diff>
--- a/data/TOPMed-studies.xlsx
+++ b/data/TOPMed-studies.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trang/PhD/Manuscripts/cardioinformatics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC897DC5-DAF0-8F4E-A2E3-556267D9A2DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE005EA-7143-F045-BB2B-A5500B9EEC9F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32060" yWindow="1140" windowWidth="43180" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32060" yWindow="1140" windowWidth="46240" windowHeight="25120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$K$1:$Q$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$K$2:$Q$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -28,7 +29,7 @@
     <author>Trang Tran</author>
   </authors>
   <commentList>
-    <comment ref="D34" authorId="0" shapeId="0" xr:uid="{13EC9BC1-D02D-0847-B02B-C98D6454CB7E}">
+    <comment ref="D35" authorId="0" shapeId="0" xr:uid="{13EC9BC1-D02D-0847-B02B-C98D6454CB7E}">
       <text>
         <r>
           <rPr>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="229">
   <si>
     <t>PI(s)</t>
   </si>
@@ -778,12 +779,21 @@
   <si>
     <t>Total sample size</t>
   </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>https://www.nhlbiwgs.org/group/project-studies</t>
+  </si>
+  <si>
+    <t>https://www.nhlbiwgs.org/group/project-studies?field_is_this_a_value=sub</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -812,6 +822,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -830,14 +855,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1175,11 +1204,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet 1" filterMode="1"/>
-  <dimension ref="A1:Q45"/>
+  <sheetPr codeName="Sheet 1"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView topLeftCell="C1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1193,182 +1222,155 @@
     <col min="12" max="12" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="M2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>220</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>223</v>
-      </c>
-      <c r="M2">
-        <v>1409</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K3" t="s">
         <v>223</v>
       </c>
       <c r="M3">
-        <v>2799</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="K4" t="s">
         <v>223</v>
       </c>
       <c r="M4">
-        <v>7500</v>
+        <v>2799</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -1380,71 +1382,68 @@
         <v>223</v>
       </c>
       <c r="M5">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" t="s">
+        <v>223</v>
+      </c>
+      <c r="M6">
         <v>1100</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>38</v>
       </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
         <v>39</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" t="s">
         <v>40</v>
-      </c>
-      <c r="I6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" t="s">
-        <v>224</v>
-      </c>
-      <c r="M6">
-        <v>15580</v>
-      </c>
-      <c r="N6">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
       </c>
       <c r="I7" t="s">
         <v>16</v>
@@ -1453,376 +1452,379 @@
         <v>224</v>
       </c>
       <c r="M7">
-        <v>1100</v>
+        <v>15580</v>
+      </c>
+      <c r="N7">
+        <v>3500</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" t="s">
+        <v>224</v>
+      </c>
+      <c r="M8">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>45</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>46</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>46</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>47</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>48</v>
       </c>
-      <c r="F8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" t="s">
         <v>223</v>
       </c>
-      <c r="M8">
+      <c r="M9">
         <f>8769+2644</f>
         <v>11413</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" t="s">
-        <v>224</v>
-      </c>
-      <c r="M9">
-        <v>958</v>
-      </c>
-    </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" t="s">
+        <v>224</v>
+      </c>
+      <c r="M10">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>53</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>54</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>54</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>55</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>56</v>
       </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
         <v>57</v>
       </c>
-      <c r="H10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" t="s">
         <v>223</v>
       </c>
-      <c r="M10">
+      <c r="M11">
         <v>3622</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" t="s">
-        <v>224</v>
-      </c>
-      <c r="M11">
-        <v>1000</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" t="s">
+        <v>224</v>
+      </c>
+      <c r="M12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>64</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>65</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>65</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>66</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>67</v>
       </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
         <v>57</v>
       </c>
-      <c r="H12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" t="s">
         <v>223</v>
       </c>
-      <c r="M12">
+      <c r="M13">
         <v>3600</v>
       </c>
     </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>68</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>69</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>69</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>70</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>71</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>72</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>73</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H14" t="s">
         <v>40</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I14" t="s">
         <v>23</v>
-      </c>
-      <c r="K13" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" t="s">
-        <v>79</v>
-      </c>
-      <c r="H14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" t="s">
-        <v>16</v>
       </c>
       <c r="K14" t="s">
         <v>224</v>
       </c>
-      <c r="M14">
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" t="s">
+        <v>224</v>
+      </c>
+      <c r="M15">
         <f>1300+5319</f>
         <v>6619</v>
       </c>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" t="s">
-        <v>224</v>
-      </c>
-      <c r="M15">
-        <v>2400</v>
-      </c>
-    </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F16" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="G16" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="K16" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="M16">
-        <v>4089</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F17" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G17" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
       </c>
       <c r="I17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K17" t="s">
         <v>223</v>
       </c>
       <c r="M17">
-        <v>1400</v>
+        <v>4089</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E18" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F18" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="G18" t="s">
         <v>28</v>
@@ -1831,36 +1833,36 @@
         <v>15</v>
       </c>
       <c r="I18" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="K18" t="s">
         <v>223</v>
       </c>
       <c r="M18">
-        <v>1860</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="H19" t="s">
         <v>15</v>
@@ -1872,505 +1874,505 @@
         <v>223</v>
       </c>
       <c r="M19">
-        <v>967</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E20" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F20" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="G20" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="H20" t="s">
         <v>15</v>
       </c>
       <c r="I20" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K20" t="s">
         <v>223</v>
       </c>
       <c r="M20">
-        <v>2270</v>
+        <v>967</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D21" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E21" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="H21" t="s">
         <v>15</v>
       </c>
       <c r="I21" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="K21" t="s">
         <v>223</v>
       </c>
       <c r="M21">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" t="s">
+        <v>223</v>
+      </c>
+      <c r="M22">
         <v>3161</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>109</v>
-      </c>
-      <c r="B22" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" t="s">
-        <v>110</v>
-      </c>
-      <c r="D22" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G22" t="s">
-        <v>28</v>
-      </c>
-      <c r="H22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" t="s">
-        <v>16</v>
-      </c>
-      <c r="K22" t="s">
-        <v>224</v>
-      </c>
-      <c r="M22">
-        <v>1500</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" t="s">
+        <v>224</v>
+      </c>
+      <c r="M23">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>113</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>114</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>114</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>115</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>116</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>117</v>
       </c>
-      <c r="G23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H23" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" t="s">
-        <v>16</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="G24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" t="s">
         <v>223</v>
       </c>
-      <c r="M23">
+      <c r="M24">
         <v>3500</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" t="s">
-        <v>118</v>
-      </c>
-      <c r="D24" t="s">
-        <v>119</v>
-      </c>
-      <c r="E24" t="s">
-        <v>120</v>
-      </c>
-      <c r="F24" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24" t="s">
-        <v>40</v>
-      </c>
-      <c r="I24" t="s">
-        <v>23</v>
-      </c>
-      <c r="K24" t="s">
-        <v>224</v>
-      </c>
-      <c r="M24">
-        <v>1548</v>
-      </c>
-      <c r="N24">
-        <v>1648</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" t="s">
+        <v>120</v>
+      </c>
+      <c r="F25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" t="s">
+        <v>224</v>
+      </c>
+      <c r="M25">
+        <v>1548</v>
+      </c>
+      <c r="N25">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>121</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>122</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>122</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>123</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
         <v>124</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
         <v>125</v>
       </c>
-      <c r="G25" t="s">
-        <v>28</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="G26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" t="s">
         <v>126</v>
       </c>
-      <c r="I25" t="s">
-        <v>16</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="I26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" t="s">
         <v>223</v>
       </c>
-      <c r="L25">
+      <c r="L26">
         <v>4595</v>
       </c>
-      <c r="M25">
+      <c r="M26">
         <v>4595</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N26" t="s">
         <v>221</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O26" t="s">
         <v>221</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P26" t="s">
         <v>221</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="Q26" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>127</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>128</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>128</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>129</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>130</v>
       </c>
-      <c r="F26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="F27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" t="s">
         <v>131</v>
       </c>
-      <c r="H26" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="H27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27" t="s">
         <v>224</v>
       </c>
-      <c r="M26">
+      <c r="M27">
         <f>2188+2959</f>
         <v>5147</v>
       </c>
     </row>
-    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>132</v>
-      </c>
-      <c r="B27" t="s">
-        <v>133</v>
-      </c>
-      <c r="C27" t="s">
-        <v>133</v>
-      </c>
-      <c r="D27" t="s">
-        <v>134</v>
-      </c>
-      <c r="E27" t="s">
-        <v>135</v>
-      </c>
-      <c r="F27" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" t="s">
-        <v>16</v>
-      </c>
-      <c r="K27" t="s">
-        <v>224</v>
-      </c>
-      <c r="M27">
-        <v>675</v>
-      </c>
-    </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" t="s">
+        <v>134</v>
+      </c>
+      <c r="E28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" t="s">
+        <v>224</v>
+      </c>
+      <c r="M28">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>136</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>137</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>137</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>138</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>139</v>
       </c>
-      <c r="F28" t="s">
-        <v>28</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="F29" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" t="s">
         <v>29</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H29" t="s">
         <v>40</v>
       </c>
-      <c r="I28" t="s">
-        <v>16</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="I29" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" t="s">
         <v>223</v>
       </c>
-      <c r="M28">
+      <c r="M29">
         <v>3230</v>
       </c>
-      <c r="N28">
+      <c r="N29">
         <v>308</v>
       </c>
     </row>
-    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>140</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>141</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>141</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>142</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>112</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>143</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G30" t="s">
         <v>22</v>
       </c>
-      <c r="H29" t="s">
-        <v>15</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="H30" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" t="s">
         <v>23</v>
-      </c>
-      <c r="K29" t="s">
-        <v>224</v>
-      </c>
-      <c r="M29">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>144</v>
-      </c>
-      <c r="B30" t="s">
-        <v>145</v>
-      </c>
-      <c r="C30" t="s">
-        <v>145</v>
-      </c>
-      <c r="D30" t="s">
-        <v>146</v>
-      </c>
-      <c r="E30" t="s">
-        <v>147</v>
-      </c>
-      <c r="F30" t="s">
-        <v>28</v>
-      </c>
-      <c r="G30" t="s">
-        <v>28</v>
-      </c>
-      <c r="H30" t="s">
-        <v>15</v>
-      </c>
-      <c r="I30" t="s">
-        <v>16</v>
       </c>
       <c r="K30" t="s">
         <v>224</v>
       </c>
       <c r="M30">
-        <v>1454</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" t="s">
+        <v>224</v>
+      </c>
+      <c r="M31">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>148</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>149</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>149</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>150</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>151</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>152</v>
       </c>
-      <c r="G31" t="s">
-        <v>28</v>
-      </c>
-      <c r="H31" t="s">
-        <v>15</v>
-      </c>
-      <c r="I31" t="s">
+      <c r="G32" t="s">
+        <v>28</v>
+      </c>
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" t="s">
         <v>23</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K32" t="s">
         <v>223</v>
       </c>
-      <c r="M31">
+      <c r="M32">
         <f>4211+3750</f>
         <v>7961</v>
       </c>
     </row>
-    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>153</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>154</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>154</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>155</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>156</v>
       </c>
-      <c r="F32" t="s">
-        <v>28</v>
-      </c>
-      <c r="G32" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32" t="s">
-        <v>15</v>
-      </c>
-      <c r="I32" t="s">
-        <v>16</v>
-      </c>
-      <c r="K32" t="s">
-        <v>224</v>
-      </c>
-      <c r="M32">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>157</v>
-      </c>
-      <c r="B33" t="s">
-        <v>158</v>
-      </c>
-      <c r="C33" t="s">
-        <v>158</v>
-      </c>
-      <c r="D33" t="s">
-        <v>159</v>
-      </c>
-      <c r="E33" t="s">
-        <v>160</v>
-      </c>
       <c r="F33" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="G33" t="s">
         <v>14</v>
@@ -2385,30 +2387,30 @@
         <v>224</v>
       </c>
       <c r="M33">
-        <v>2809</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B34" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C34" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D34" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E34" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F34" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G34" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="H34" t="s">
         <v>15</v>
@@ -2420,30 +2422,30 @@
         <v>224</v>
       </c>
       <c r="M34">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+        <v>2809</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B35" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C35" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D35" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E35" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F35" t="s">
-        <v>13</v>
+        <v>166</v>
       </c>
       <c r="G35" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="H35" t="s">
         <v>15</v>
@@ -2455,30 +2457,30 @@
         <v>224</v>
       </c>
       <c r="M35">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B36" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C36" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D36" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E36" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F36" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="H36" t="s">
         <v>15</v>
@@ -2490,349 +2492,399 @@
         <v>224</v>
       </c>
       <c r="M36">
-        <v>1900</v>
+        <v>650</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>171</v>
+      </c>
+      <c r="B37" t="s">
+        <v>172</v>
+      </c>
+      <c r="C37" t="s">
+        <v>172</v>
+      </c>
+      <c r="D37" t="s">
+        <v>173</v>
+      </c>
+      <c r="E37" t="s">
+        <v>174</v>
+      </c>
+      <c r="F37" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" t="s">
+        <v>16</v>
+      </c>
+      <c r="K37" t="s">
+        <v>224</v>
+      </c>
+      <c r="M37">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>175</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>176</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>176</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>177</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>178</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F38" t="s">
         <v>179</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G38" t="s">
         <v>180</v>
       </c>
-      <c r="H37" t="s">
-        <v>15</v>
-      </c>
-      <c r="I37" t="s">
-        <v>16</v>
-      </c>
-      <c r="K37" t="s">
+      <c r="H38" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" t="s">
+        <v>16</v>
+      </c>
+      <c r="K38" t="s">
         <v>223</v>
       </c>
-      <c r="M37">
+      <c r="M38">
         <f>384+912</f>
         <v>1296</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>181</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>182</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>182</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>183</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>184</v>
       </c>
-      <c r="F38" t="s">
-        <v>28</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="F39" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" t="s">
         <v>185</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H39" t="s">
         <v>40</v>
       </c>
-      <c r="I38" t="s">
-        <v>28</v>
-      </c>
-      <c r="K38" t="s">
+      <c r="I39" t="s">
+        <v>28</v>
+      </c>
+      <c r="K39" t="s">
         <v>223</v>
       </c>
-      <c r="M38">
+      <c r="M39">
         <v>1500</v>
       </c>
-      <c r="N38">
+      <c r="N39">
         <v>450</v>
       </c>
     </row>
-    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>186</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>187</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>188</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>189</v>
       </c>
-      <c r="E39" t="s">
-        <v>28</v>
-      </c>
-      <c r="F39" t="s">
-        <v>28</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="E40" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" t="s">
         <v>14</v>
       </c>
-      <c r="H39" t="s">
-        <v>15</v>
-      </c>
-      <c r="I39" t="s">
+      <c r="H40" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" t="s">
         <v>23</v>
-      </c>
-      <c r="K39" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>171</v>
-      </c>
-      <c r="B40" t="s">
-        <v>190</v>
-      </c>
-      <c r="C40" t="s">
-        <v>190</v>
-      </c>
-      <c r="D40" t="s">
-        <v>191</v>
-      </c>
-      <c r="E40" t="s">
-        <v>192</v>
-      </c>
-      <c r="F40" t="s">
-        <v>28</v>
-      </c>
-      <c r="G40" t="s">
-        <v>29</v>
-      </c>
-      <c r="H40" t="s">
-        <v>40</v>
-      </c>
-      <c r="I40" t="s">
-        <v>193</v>
       </c>
       <c r="K40" t="s">
         <v>224</v>
       </c>
-      <c r="M40">
-        <v>2981</v>
-      </c>
-      <c r="N40">
-        <v>5253</v>
-      </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="B41" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C41" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D41" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E41" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F41" t="s">
-        <v>198</v>
+        <v>28</v>
       </c>
       <c r="G41" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H41" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="I41" t="s">
-        <v>16</v>
+        <v>193</v>
       </c>
       <c r="K41" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="M41">
-        <v>2585</v>
+        <v>2981</v>
+      </c>
+      <c r="N41">
+        <v>5253</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B42" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C42" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D42" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E42" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F42" t="s">
-        <v>28</v>
+        <v>198</v>
       </c>
       <c r="G42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H42" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="I42" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K42" t="s">
         <v>223</v>
       </c>
       <c r="M42">
-        <v>1078</v>
-      </c>
-      <c r="N42">
-        <v>1078</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B43" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C43" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D43" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E43" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F43" t="s">
         <v>28</v>
       </c>
       <c r="G43" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="H43" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="I43" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="K43" t="s">
         <v>223</v>
       </c>
       <c r="M43">
+        <v>1078</v>
+      </c>
+      <c r="N43">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>203</v>
+      </c>
+      <c r="B44" t="s">
+        <v>204</v>
+      </c>
+      <c r="C44" t="s">
+        <v>204</v>
+      </c>
+      <c r="D44" t="s">
+        <v>205</v>
+      </c>
+      <c r="E44" t="s">
+        <v>206</v>
+      </c>
+      <c r="F44" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" t="s">
+        <v>16</v>
+      </c>
+      <c r="K44" t="s">
+        <v>223</v>
+      </c>
+      <c r="M44">
         <v>6000</v>
       </c>
     </row>
-    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>207</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>208</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>208</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>209</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>210</v>
       </c>
-      <c r="F44" t="s">
-        <v>28</v>
-      </c>
-      <c r="G44" t="s">
-        <v>28</v>
-      </c>
-      <c r="H44" t="s">
-        <v>15</v>
-      </c>
-      <c r="I44" t="s">
-        <v>16</v>
-      </c>
-      <c r="K44" t="s">
-        <v>224</v>
-      </c>
-      <c r="M44">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>211</v>
-      </c>
-      <c r="B45" t="s">
-        <v>212</v>
-      </c>
-      <c r="C45" t="s">
-        <v>212</v>
-      </c>
-      <c r="D45" t="s">
-        <v>213</v>
-      </c>
-      <c r="E45" t="s">
-        <v>214</v>
-      </c>
       <c r="F45" t="s">
         <v>28</v>
       </c>
       <c r="G45" t="s">
-        <v>215</v>
+        <v>28</v>
       </c>
       <c r="H45" t="s">
-        <v>216</v>
+        <v>15</v>
       </c>
       <c r="I45" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K45" t="s">
         <v>224</v>
       </c>
       <c r="M45">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>211</v>
+      </c>
+      <c r="B46" t="s">
+        <v>212</v>
+      </c>
+      <c r="C46" t="s">
+        <v>212</v>
+      </c>
+      <c r="D46" t="s">
+        <v>213</v>
+      </c>
+      <c r="E46" t="s">
+        <v>214</v>
+      </c>
+      <c r="F46" t="s">
+        <v>28</v>
+      </c>
+      <c r="G46" t="s">
+        <v>215</v>
+      </c>
+      <c r="H46" t="s">
+        <v>216</v>
+      </c>
+      <c r="I46" t="s">
+        <v>23</v>
+      </c>
+      <c r="K46" t="s">
+        <v>223</v>
+      </c>
+      <c r="M46">
         <v>11100</v>
       </c>
-      <c r="N45">
+      <c r="N46">
         <v>1400</v>
       </c>
-      <c r="O45">
+      <c r="O46">
         <v>1400</v>
       </c>
-      <c r="P45">
+      <c r="P46">
         <v>1400</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="K1:Q45" xr:uid="{E3B980D6-A070-E044-A82C-5F255BE8C974}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="yes"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="K2:Q46" xr:uid="{E3B980D6-A070-E044-A82C-5F255BE8C974}"/>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1" xr:uid="{12765C41-700A-454C-9606-BA4EFC204530}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C042D7FF-FB75-514F-BDD8-A67C31447E95}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>